<commit_message>
minor comment changes & document finished
</commit_message>
<xml_diff>
--- a/algo/mp3/doc/data.xlsx
+++ b/algo/mp3/doc/data.xlsx
@@ -8,20 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ohgree/Library/Mobile Documents/com~apple~CloudDocs/sogang/sem4/cs2019-2/algo/mp3/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3674386-C71D-8248-9C12-1809115D042B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90668A29-146E-5846-BC91-EB7EFB7BD7F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-100" yWindow="460" windowWidth="28300" windowHeight="16520" xr2:uid="{556B446E-33C3-5F49-AB81-504AE16EC2E3}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28300" windowHeight="16520" xr2:uid="{556B446E-33C3-5F49-AB81-504AE16EC2E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v2.0" hidden="1">Sheet1!$H$1</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">Sheet1!$H$2</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">Sheet1!$I$1:$L$1</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">Sheet1!$I$2:$L$2</definedName>
-  </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -80,7 +74,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="179" formatCode="General\ &quot;Bytes&quot;"/>
+    <numFmt numFmtId="176" formatCode="General\ &quot;Bytes&quot;"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -139,7 +133,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -241,7 +235,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$2</c:f>
+              <c:f>Sheet1!$H$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -262,7 +256,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$I$1:$L$1</c:f>
+              <c:f>Sheet1!$I$2:$L$2</c:f>
               <c:numCache>
                 <c:formatCode>General\ "Bytes"</c:formatCode>
                 <c:ptCount val="4"/>
@@ -283,7 +277,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$2:$L$2</c:f>
+              <c:f>Sheet1!$I$3:$L$3</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1359,11 +1353,13 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1384,104 +1380,124 @@
       <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2">
-        <f t="shared" ref="I1:L1" si="0">B2</f>
-        <v>508</v>
-      </c>
-      <c r="J1" s="2">
+      <c r="I1" s="2" t="str">
+        <f>B1</f>
+        <v>lorem0.txt</v>
+      </c>
+      <c r="J1" s="2" t="str">
+        <f t="shared" ref="J1:L1" si="0">C1</f>
+        <v>lorem1.txt</v>
+      </c>
+      <c r="K1" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>60185</v>
-      </c>
-      <c r="K1" s="2">
+        <v>lorem2.txt</v>
+      </c>
+      <c r="L1" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>902775</v>
-      </c>
-      <c r="L1" s="2">
-        <f t="shared" si="0"/>
-        <v>12639060</v>
+        <v>lorem3.txt</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>508</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>60185</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>902775</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>12639060</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>128000</v>
       </c>
-      <c r="H2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="1">
-        <f t="shared" ref="I2:L2" si="1">B4</f>
-        <v>1.6377952755905512</v>
-      </c>
-      <c r="J2" s="1">
-        <f t="shared" si="1"/>
-        <v>0.5465647586607959</v>
-      </c>
-      <c r="K2" s="1">
-        <f t="shared" si="1"/>
-        <v>0.53544017058514026</v>
-      </c>
-      <c r="L2" s="1">
-        <f t="shared" si="1"/>
-        <v>0.53470978063242047</v>
+      <c r="H2" s="2" t="str">
+        <f>A2</f>
+        <v>raw</v>
+      </c>
+      <c r="I2" s="2">
+        <f>B2</f>
+        <v>508</v>
+      </c>
+      <c r="J2" s="2">
+        <f>C2</f>
+        <v>60185</v>
+      </c>
+      <c r="K2" s="2">
+        <f>D2</f>
+        <v>902775</v>
+      </c>
+      <c r="L2" s="2">
+        <f>E2</f>
+        <v>12639060</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>832</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>32895</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>483382</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>6758229</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <v>114179</v>
+      </c>
+      <c r="H3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="1">
+        <f>B4</f>
+        <v>1.6377952755905512</v>
+      </c>
+      <c r="J3" s="1">
+        <f>C4</f>
+        <v>0.5465647586607959</v>
+      </c>
+      <c r="K3" s="1">
+        <f>D4</f>
+        <v>0.53544017058514026</v>
+      </c>
+      <c r="L3" s="1">
+        <f>E4</f>
+        <v>0.53470978063242047</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <f>(B3/B2)</f>
         <v>1.6377952755905512</v>
       </c>
-      <c r="C4">
-        <f t="shared" ref="C4:F4" si="2">(C3/C2)</f>
+      <c r="C4" s="1">
+        <f t="shared" ref="C4:F4" si="1">(C3/C2)</f>
         <v>0.5465647586607959</v>
       </c>
-      <c r="D4">
-        <f t="shared" si="2"/>
+      <c r="D4" s="1">
+        <f t="shared" si="1"/>
         <v>0.53544017058514026</v>
       </c>
-      <c r="E4">
-        <f t="shared" si="2"/>
+      <c r="E4" s="1">
+        <f t="shared" si="1"/>
         <v>0.53470978063242047</v>
       </c>
-      <c r="F4">
-        <f t="shared" si="2"/>
+      <c r="F4" s="1">
+        <f t="shared" si="1"/>
         <v>0.89202343750000002</v>
       </c>
     </row>

</xml_diff>

<commit_message>
MP3 finished & verified
</commit_message>
<xml_diff>
--- a/algo/mp3/doc/data.xlsx
+++ b/algo/mp3/doc/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ohgree/Library/Mobile Documents/com~apple~CloudDocs/sogang/sem4/cs2019-2/algo/mp3/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90668A29-146E-5846-BC91-EB7EFB7BD7F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4FEAA5-127F-B948-9D5B-3412E3152DE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28300" windowHeight="16520" xr2:uid="{556B446E-33C3-5F49-AB81-504AE16EC2E3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>raw</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -66,6 +66,10 @@
   </si>
   <si>
     <t>ratio</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>worst case</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1350,10 +1354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C20C398-B9A8-374C-99A9-7CF4CA7B1C7C}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -1501,6 +1505,36 @@
         <v>0.89202343750000002</v>
       </c>
     </row>
+    <row r="10" spans="1:12">
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2">
+        <v>128000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2">
+        <v>114179</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="1">
+        <f t="shared" ref="C13" si="2">(C12/C11)</f>
+        <v>0.89202343750000002</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>